<commit_message>
Promena specifikacije za potenciometar, 06.06.2020
</commit_message>
<xml_diff>
--- a/BOM_Signal_Generator_Verzija_TH.xlsx
+++ b/BOM_Signal_Generator_Verzija_TH.xlsx
@@ -225,9 +225,6 @@
     <t>75-MKP1839447161</t>
   </si>
   <si>
-    <t xml:space="preserve">858-P0925NFC15BR20K </t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -612,6 +609,9 @@
   </si>
   <si>
     <t>Total with VAT</t>
+  </si>
+  <si>
+    <t>652-3310H-001-203L</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1035,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1123,6 +1123,14 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1132,17 +1140,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1450,8 +1451,8 @@
   </sheetPr>
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,16 +1468,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="41"/>
+      <c r="A1" s="43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1495,13 +1496,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1509,16 +1510,16 @@
         <v>38</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="7">
         <v>5.9</v>
@@ -1528,7 +1529,7 @@
         <v>5.9</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1536,16 +1537,16 @@
         <v>56</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="11">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="11">
         <v>6.17</v>
@@ -1555,24 +1556,24 @@
         <v>6.17</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>87</v>
-      </c>
       <c r="C5" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D5" s="11">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F5" s="11">
         <v>8.17</v>
@@ -1582,15 +1583,15 @@
         <v>8.17</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>141</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>49</v>
@@ -1599,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6" s="11">
         <v>1.43</v>
@@ -1612,7 +1613,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>13</v>
@@ -1624,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="11">
         <v>0.52400000000000002</v>
@@ -1637,7 +1638,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>25</v>
@@ -1662,10 +1663,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>49</v>
@@ -1674,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F9" s="15">
         <v>1.2</v>
@@ -1687,19 +1688,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="C10" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="D10" s="11">
-        <v>1</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="F10" s="15">
         <v>3.46</v>
@@ -1712,7 +1713,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>24</v>
@@ -1737,10 +1738,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>51</v>
@@ -1749,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="11">
         <v>0.38</v>
@@ -1783,7 +1784,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>34</v>
@@ -1808,7 +1809,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>36</v>
@@ -1833,13 +1834,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="11">
         <v>2</v>
@@ -1882,7 +1883,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>58</v>
@@ -1891,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F18" s="11">
         <v>1.45</v>
@@ -1904,44 +1905,44 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>68</v>
+      <c r="E19" s="47" t="s">
+        <v>192</v>
       </c>
       <c r="F19" s="11">
-        <v>2.71</v>
+        <v>6.72</v>
       </c>
       <c r="G19" s="12">
         <f t="shared" si="0"/>
-        <v>2.71</v>
+        <v>6.72</v>
       </c>
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="11">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" s="11">
         <v>1.05</v>
@@ -1951,12 +1952,12 @@
         <v>1.05</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B21" s="11">
         <v>200</v>
@@ -1981,7 +1982,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>17</v>
@@ -1993,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="11">
         <v>1.41</v>
@@ -2006,7 +2007,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B23" s="11">
         <v>500</v>
@@ -2018,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="11">
         <v>1.39</v>
@@ -2031,13 +2032,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" s="11">
         <v>2</v>
@@ -2052,13 +2053,13 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="11">
         <v>100</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="11">
         <v>4</v>
@@ -2073,13 +2074,13 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="11">
         <v>2</v>
@@ -2094,13 +2095,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="11">
         <v>2</v>
@@ -2115,13 +2116,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="11">
         <v>1</v>
@@ -2142,7 +2143,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="11">
         <v>1</v>
@@ -2160,10 +2161,10 @@
         <v>16</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="11">
         <v>1</v>
@@ -2178,13 +2179,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" s="11">
         <v>510</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="11">
         <v>7</v>
@@ -2199,13 +2200,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="11">
         <v>4</v>
@@ -2220,13 +2221,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="11">
         <v>1</v>
@@ -2241,13 +2242,13 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="11" t="s">
-        <v>158</v>
-      </c>
       <c r="C34" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="11">
         <v>2</v>
@@ -2262,13 +2263,13 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="11">
         <v>2</v>
@@ -2283,13 +2284,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="11">
         <v>1</v>
@@ -2304,13 +2305,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D37" s="11">
         <v>1</v>
@@ -2325,13 +2326,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D38" s="11">
         <v>1</v>
@@ -2346,13 +2347,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D39" s="11">
         <v>1</v>
@@ -2367,13 +2368,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D40" s="11">
         <v>1</v>
@@ -2388,13 +2389,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D41" s="11">
         <v>2</v>
@@ -2412,10 +2413,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D42" s="11">
         <v>1</v>
@@ -2433,10 +2434,10 @@
         <v>37</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D43" s="11">
         <v>1</v>
@@ -2451,13 +2452,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B44" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D44" s="11">
         <v>1</v>
@@ -2472,13 +2473,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>152</v>
-      </c>
       <c r="C45" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D45" s="11">
         <v>1</v>
@@ -2493,13 +2494,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D46" s="11">
         <v>4</v>
@@ -2514,13 +2515,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B47" s="11">
         <v>62</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D47" s="11">
         <v>1</v>
@@ -2535,13 +2536,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B48" s="11">
         <v>56</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D48" s="11">
         <v>1</v>
@@ -2656,7 +2657,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="11" t="s">
         <v>19</v>
@@ -2674,12 +2675,12 @@
         <v>0</v>
       </c>
       <c r="H53" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" s="11" t="s">
         <v>28</v>
@@ -2697,24 +2698,24 @@
         <v>0</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B55" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="11" t="s">
-        <v>170</v>
-      </c>
       <c r="D55" s="11">
         <v>1</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F55" s="11">
         <v>0.52</v>
@@ -2724,24 +2725,24 @@
         <v>0.52</v>
       </c>
       <c r="H55" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D56" s="11">
+        <v>1</v>
+      </c>
+      <c r="E56" s="21" t="s">
         <v>170</v>
-      </c>
-      <c r="D56" s="11">
-        <v>1</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>171</v>
       </c>
       <c r="F56" s="11">
         <v>1.23</v>
@@ -2751,12 +2752,12 @@
         <v>1.23</v>
       </c>
       <c r="H56" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>63</v>
@@ -2768,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F57" s="11">
         <v>0.4</v>
@@ -2781,7 +2782,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>4</v>
@@ -2793,7 +2794,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F58" s="11">
         <v>0.27100000000000002</v>
@@ -2806,10 +2807,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" s="11" t="s">
         <v>52</v>
@@ -2818,7 +2819,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F59" s="11">
         <v>0.32300000000000001</v>
@@ -2831,13 +2832,13 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B60" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>97</v>
-      </c>
-      <c r="C60" s="11" t="s">
-        <v>98</v>
       </c>
       <c r="D60" s="11">
         <v>1</v>
@@ -2849,18 +2850,18 @@
         <v>0</v>
       </c>
       <c r="H60" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" s="23">
         <v>11</v>
@@ -2872,18 +2873,18 @@
         <v>0</v>
       </c>
       <c r="H61" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B62" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D62" s="11">
         <v>1</v>
@@ -2895,24 +2896,24 @@
         <v>0</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A63" s="25" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D63" s="26">
         <v>10</v>
       </c>
       <c r="E63" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F63" s="26">
         <v>0.08</v>
@@ -2922,18 +2923,18 @@
         <v>0.8</v>
       </c>
       <c r="H63" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="B64" s="26" t="s">
-        <v>178</v>
-      </c>
       <c r="C64" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D64" s="26">
         <v>2</v>
@@ -2942,18 +2943,18 @@
       <c r="F64" s="26"/>
       <c r="G64" s="27"/>
       <c r="H64" s="20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="B65" s="26" t="s">
-        <v>183</v>
-      </c>
       <c r="C65" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D65" s="26">
         <v>1</v>
@@ -2962,18 +2963,18 @@
       <c r="F65" s="26"/>
       <c r="G65" s="27"/>
       <c r="H65" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B66" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="B66" s="29" t="s">
-        <v>181</v>
-      </c>
       <c r="C66" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D66" s="29">
         <v>1</v>
@@ -2985,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2995,32 +2996,32 @@
       <c r="D67" s="34"/>
       <c r="E67" s="35"/>
       <c r="F67" s="36" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G67" s="37">
         <f>SUM(G3:G66)</f>
-        <v>62.548999999999999</v>
+        <v>66.558999999999997</v>
       </c>
       <c r="H67" s="38"/>
     </row>
     <row r="68" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="42"/>
-      <c r="B68" s="43"/>
-      <c r="C68" s="44" t="s">
+      <c r="A68" s="39"/>
+      <c r="B68" s="40"/>
+      <c r="C68" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="D68" s="46"/>
+      <c r="E68" s="41">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F68" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="D68" s="44"/>
-      <c r="E68" s="45">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="F68" s="43" t="s">
-        <v>192</v>
-      </c>
-      <c r="G68" s="46">
+      <c r="G68" s="42">
         <f>G67*(1+E68)</f>
-        <v>67.365273000000002</v>
-      </c>
-      <c r="H68" s="42"/>
+        <v>71.684042999999988</v>
+      </c>
+      <c r="H68" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>